<commit_message>
this project might take a while: introduced job classes
</commit_message>
<xml_diff>
--- a/urls.xlsx
+++ b/urls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hitae\OneDrive\Documents\GitHub\fintech_scraper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B82BDC-613D-4352-945A-13028EED3CE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFEDE382-15AE-4A61-823A-A1839EAFDDD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10" yWindow="10" windowWidth="19190" windowHeight="11270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Hudson River Trading</t>
   </si>
@@ -33,23 +33,50 @@
     <t>https://www.hudsonrivertrading.com/careers/#newjobsboard</t>
   </si>
   <si>
-    <t>Names</t>
-  </si>
-  <si>
-    <t>Careers</t>
-  </si>
-  <si>
-    <t>Base</t>
-  </si>
-  <si>
     <t>https://www.hudsonrivertrading.com/</t>
+  </si>
+  <si>
+    <t>names</t>
+  </si>
+  <si>
+    <t>careers</t>
+  </si>
+  <si>
+    <t>base</t>
+  </si>
+  <si>
+    <t>job-title</t>
+  </si>
+  <si>
+    <t>Jump Trading</t>
+  </si>
+  <si>
+    <t>https://www.jumptrading.com/careers/</t>
+  </si>
+  <si>
+    <t>https://www.jumptrading.com/</t>
+  </si>
+  <si>
+    <t>job-location-name</t>
+  </si>
+  <si>
+    <t>text-xl lg:text-2xl font-medium text-black group-hover:text-jump-red</t>
+  </si>
+  <si>
+    <t>text-base lg:text-lg text-dark-gray group-hover:text-black</t>
+  </si>
+  <si>
+    <t>job_classes</t>
+  </si>
+  <si>
+    <t>location_classes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -61,6 +88,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -87,9 +120,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -371,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -382,20 +418,28 @@
     <col min="1" max="1" width="22.26953125" customWidth="1"/>
     <col min="2" max="2" width="52.6796875" customWidth="1"/>
     <col min="3" max="3" width="32.40625" customWidth="1"/>
+    <col min="4" max="4" width="21.40625" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -403,7 +447,30 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="59" x14ac:dyDescent="0.75">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Testing + Message Sending
Did lots of testing. Didn't feel like working with nested HTML classes so decided to work on message sending instead. SMS costs money no matter what, so decided to go with whatsapp. So far, the library I am using seems pretty buggy but I can worry about that later. Message sending seems to work based on prelim testing, but not receiving notifications on phone. Might need to create a separate whatsapp account for this.
</commit_message>
<xml_diff>
--- a/urls.xlsx
+++ b/urls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hitae\OneDrive\Documents\GitHub\fintech_scraper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFEDE382-15AE-4A61-823A-A1839EAFDDD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{222D799A-6247-4D8D-B850-5D5E7138386C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10" yWindow="10" windowWidth="19190" windowHeight="11270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Hudson River Trading</t>
   </si>
@@ -70,6 +70,18 @@
   </si>
   <si>
     <t>location_classes</t>
+  </si>
+  <si>
+    <t>Susquehanna</t>
+  </si>
+  <si>
+    <t>job-location</t>
+  </si>
+  <si>
+    <t>https://sig.com/</t>
+  </si>
+  <si>
+    <t>https://careers.sig.com/c/quantitative-trading-strategy-jobs</t>
   </si>
 </sst>
 </file>
@@ -407,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -473,6 +485,23 @@
         <v>12</v>
       </c>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" location="newjobsboard" xr:uid="{2AED68D4-A551-45AC-A853-437243CDA450}"/>

</xml_diff>

<commit_message>
still can't get nested tags to work, will probably work on location now
</commit_message>
<xml_diff>
--- a/urls.xlsx
+++ b/urls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hitae\OneDrive\Documents\GitHub\fintech_scraper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{222D799A-6247-4D8D-B850-5D5E7138386C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EE8E5A4-4D55-4088-A0A2-63086FAD20C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10" yWindow="10" windowWidth="19190" windowHeight="11270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -422,7 +422,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>

</xml_diff>

<commit_message>
Added Multiple Page Support
So the commit message is kind of a lie. Instead of adding support to "scroll" through several pages of a career website, I decided to use the 'filtered" url for the websites that require scrolling through multipl pages (i.e imc). However, it didn't work right off the bat, so I had to use selenium to parse the webpage. I think this is because the url redirect is happening in the actual JS code (I could be wring tho). This made it a bit slower, but we shall see how this goes. Still can't figure out nested HTML classes tho
</commit_message>
<xml_diff>
--- a/urls.xlsx
+++ b/urls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hitae\OneDrive\Documents\GitHub\fintech_scraper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EE8E5A4-4D55-4088-A0A2-63086FAD20C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81646F34-4382-40AA-B946-6280D32DCE63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10" yWindow="10" windowWidth="19190" windowHeight="11270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Hudson River Trading</t>
   </si>
@@ -82,6 +82,21 @@
   </si>
   <si>
     <t>https://careers.sig.com/c/quantitative-trading-strategy-jobs</t>
+  </si>
+  <si>
+    <t>IMC</t>
+  </si>
+  <si>
+    <t>_13fp8yk6c dzswju0 dzswjuc ryl3ea0 ajj7g52 _1e5s7rk1</t>
+  </si>
+  <si>
+    <t>https://www.imc.com/us/</t>
+  </si>
+  <si>
+    <t>_13fp8yk6c dzswju0 dzswju5</t>
+  </si>
+  <si>
+    <t>https://www.imc.com/us/search-careers?jobTypes=Intern&amp;page=1</t>
   </si>
 </sst>
 </file>
@@ -132,10 +147,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -419,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -451,56 +471,423 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="59" x14ac:dyDescent="0.75">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="2" t="s">
         <v>16</v>
       </c>
+    </row>
+    <row r="5" spans="1:5" ht="44.25" x14ac:dyDescent="0.75">
+      <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A52" s="2"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A54" s="2"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A55" s="2"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>